<commit_message>
Metadata on sWord levels.
</commit_message>
<xml_diff>
--- a/R_files/Rresults/matrices/metadata_sWord_levels_Jan242016.xlsx
+++ b/R_files/Rresults/matrices/metadata_sWord_levels_Jan242016.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="45">
   <si>
     <t>Athenaeus</t>
   </si>
@@ -129,6 +129,36 @@
   </si>
   <si>
     <t>&lt;sWord-10&gt;</t>
+  </si>
+  <si>
+    <t>&lt;sWord-11&gt;</t>
+  </si>
+  <si>
+    <t>&lt;sWord-12&gt;</t>
+  </si>
+  <si>
+    <t>&lt;sWord-13&gt;</t>
+  </si>
+  <si>
+    <t>&lt;sWord-14&gt;</t>
+  </si>
+  <si>
+    <t>&lt;sWord-15&gt;</t>
+  </si>
+  <si>
+    <t>&lt;sWord-16&gt;</t>
+  </si>
+  <si>
+    <t>&lt;sWord-17&gt;</t>
+  </si>
+  <si>
+    <t>&lt;sWord-18&gt;</t>
+  </si>
+  <si>
+    <t>&lt;sWord-19&gt;</t>
+  </si>
+  <si>
+    <t>&lt;sWord-20&gt;</t>
   </si>
 </sst>
 </file>
@@ -474,10 +504,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P20"/>
+  <dimension ref="A1:X20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="W22" sqref="W22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -485,9 +518,14 @@
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="10" width="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="12" bestFit="1" customWidth="1"/>
+    <col min="15" max="19" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="24" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>23</v>
       </c>
@@ -524,8 +562,38 @@
       <c r="N1" t="s">
         <v>34</v>
       </c>
+      <c r="O1" t="s">
+        <v>35</v>
+      </c>
+      <c r="P1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>37</v>
+      </c>
+      <c r="R1" t="s">
+        <v>38</v>
+      </c>
+      <c r="S1" t="s">
+        <v>39</v>
+      </c>
+      <c r="T1" t="s">
+        <v>40</v>
+      </c>
+      <c r="U1" t="s">
+        <v>41</v>
+      </c>
+      <c r="V1" t="s">
+        <v>42</v>
+      </c>
+      <c r="W1" t="s">
+        <v>43</v>
+      </c>
+      <c r="X1" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -568,8 +636,38 @@
       <c r="N2">
         <v>355</v>
       </c>
+      <c r="O2">
+        <v>185</v>
+      </c>
+      <c r="P2">
+        <v>82</v>
+      </c>
+      <c r="Q2">
+        <v>42</v>
+      </c>
+      <c r="R2">
+        <v>22</v>
+      </c>
+      <c r="S2">
+        <v>13</v>
+      </c>
+      <c r="T2">
+        <v>8</v>
+      </c>
+      <c r="U2">
+        <v>4</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -612,8 +710,38 @@
       <c r="N3">
         <v>166</v>
       </c>
+      <c r="O3">
+        <v>72</v>
+      </c>
+      <c r="P3">
+        <v>26</v>
+      </c>
+      <c r="Q3">
+        <v>5</v>
+      </c>
+      <c r="R3">
+        <v>1</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="U3">
+        <v>0</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <v>0</v>
+      </c>
+      <c r="X3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -656,8 +784,38 @@
       <c r="N4">
         <v>228</v>
       </c>
+      <c r="O4">
+        <v>99</v>
+      </c>
+      <c r="P4">
+        <v>40</v>
+      </c>
+      <c r="Q4">
+        <v>14</v>
+      </c>
+      <c r="R4">
+        <v>8</v>
+      </c>
+      <c r="S4">
+        <v>4</v>
+      </c>
+      <c r="T4">
+        <v>2</v>
+      </c>
+      <c r="U4">
+        <v>0</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <v>0</v>
+      </c>
+      <c r="X4">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -700,8 +858,38 @@
       <c r="N5">
         <v>352</v>
       </c>
+      <c r="O5">
+        <v>189</v>
+      </c>
+      <c r="P5">
+        <v>87</v>
+      </c>
+      <c r="Q5">
+        <v>60</v>
+      </c>
+      <c r="R5">
+        <v>39</v>
+      </c>
+      <c r="S5">
+        <v>16</v>
+      </c>
+      <c r="T5">
+        <v>7</v>
+      </c>
+      <c r="U5">
+        <v>1</v>
+      </c>
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5">
+        <v>0</v>
+      </c>
+      <c r="X5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -744,8 +932,38 @@
       <c r="N6">
         <v>141</v>
       </c>
+      <c r="O6">
+        <v>82</v>
+      </c>
+      <c r="P6">
+        <v>43</v>
+      </c>
+      <c r="Q6">
+        <v>23</v>
+      </c>
+      <c r="R6">
+        <v>15</v>
+      </c>
+      <c r="S6">
+        <v>8</v>
+      </c>
+      <c r="T6">
+        <v>3</v>
+      </c>
+      <c r="U6">
+        <v>0</v>
+      </c>
+      <c r="V6">
+        <v>0</v>
+      </c>
+      <c r="W6">
+        <v>0</v>
+      </c>
+      <c r="X6">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -788,8 +1006,38 @@
       <c r="N7">
         <v>141</v>
       </c>
+      <c r="O7">
+        <v>78</v>
+      </c>
+      <c r="P7">
+        <v>47</v>
+      </c>
+      <c r="Q7">
+        <v>38</v>
+      </c>
+      <c r="R7">
+        <v>28</v>
+      </c>
+      <c r="S7">
+        <v>20</v>
+      </c>
+      <c r="T7">
+        <v>12</v>
+      </c>
+      <c r="U7">
+        <v>6</v>
+      </c>
+      <c r="V7">
+        <v>3</v>
+      </c>
+      <c r="W7">
+        <v>1</v>
+      </c>
+      <c r="X7">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -832,8 +1080,38 @@
       <c r="N8">
         <v>48</v>
       </c>
+      <c r="O8">
+        <v>26</v>
+      </c>
+      <c r="P8">
+        <v>13</v>
+      </c>
+      <c r="Q8">
+        <v>4</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8">
+        <v>0</v>
+      </c>
+      <c r="T8">
+        <v>0</v>
+      </c>
+      <c r="U8">
+        <v>0</v>
+      </c>
+      <c r="V8">
+        <v>0</v>
+      </c>
+      <c r="W8">
+        <v>0</v>
+      </c>
+      <c r="X8">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -876,8 +1154,38 @@
       <c r="N9">
         <v>28</v>
       </c>
+      <c r="O9">
+        <v>16</v>
+      </c>
+      <c r="P9">
+        <v>8</v>
+      </c>
+      <c r="Q9">
+        <v>3</v>
+      </c>
+      <c r="R9">
+        <v>0</v>
+      </c>
+      <c r="S9">
+        <v>0</v>
+      </c>
+      <c r="T9">
+        <v>0</v>
+      </c>
+      <c r="U9">
+        <v>0</v>
+      </c>
+      <c r="V9">
+        <v>0</v>
+      </c>
+      <c r="W9">
+        <v>0</v>
+      </c>
+      <c r="X9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -920,8 +1228,38 @@
       <c r="N10">
         <v>285</v>
       </c>
+      <c r="O10">
+        <v>152</v>
+      </c>
+      <c r="P10">
+        <v>73</v>
+      </c>
+      <c r="Q10">
+        <v>45</v>
+      </c>
+      <c r="R10">
+        <v>29</v>
+      </c>
+      <c r="S10">
+        <v>13</v>
+      </c>
+      <c r="T10">
+        <v>4</v>
+      </c>
+      <c r="U10">
+        <v>0</v>
+      </c>
+      <c r="V10">
+        <v>0</v>
+      </c>
+      <c r="W10">
+        <v>0</v>
+      </c>
+      <c r="X10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -964,8 +1302,38 @@
       <c r="N11">
         <v>185</v>
       </c>
+      <c r="O11">
+        <v>100</v>
+      </c>
+      <c r="P11">
+        <v>45</v>
+      </c>
+      <c r="Q11">
+        <v>15</v>
+      </c>
+      <c r="R11">
+        <v>5</v>
+      </c>
+      <c r="S11">
+        <v>2</v>
+      </c>
+      <c r="T11">
+        <v>0</v>
+      </c>
+      <c r="U11">
+        <v>0</v>
+      </c>
+      <c r="V11">
+        <v>0</v>
+      </c>
+      <c r="W11">
+        <v>0</v>
+      </c>
+      <c r="X11">
+        <v>0</v>
+      </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
@@ -1008,8 +1376,38 @@
       <c r="N12">
         <v>432</v>
       </c>
+      <c r="O12">
+        <v>174</v>
+      </c>
+      <c r="P12">
+        <v>71</v>
+      </c>
+      <c r="Q12">
+        <v>33</v>
+      </c>
+      <c r="R12">
+        <v>18</v>
+      </c>
+      <c r="S12">
+        <v>5</v>
+      </c>
+      <c r="T12">
+        <v>1</v>
+      </c>
+      <c r="U12">
+        <v>0</v>
+      </c>
+      <c r="V12">
+        <v>0</v>
+      </c>
+      <c r="W12">
+        <v>0</v>
+      </c>
+      <c r="X12">
+        <v>0</v>
+      </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
@@ -1052,8 +1450,38 @@
       <c r="N13">
         <v>470</v>
       </c>
+      <c r="O13">
+        <v>266</v>
+      </c>
+      <c r="P13">
+        <v>159</v>
+      </c>
+      <c r="Q13">
+        <v>90</v>
+      </c>
+      <c r="R13">
+        <v>55</v>
+      </c>
+      <c r="S13">
+        <v>26</v>
+      </c>
+      <c r="T13">
+        <v>14</v>
+      </c>
+      <c r="U13">
+        <v>5</v>
+      </c>
+      <c r="V13">
+        <v>1</v>
+      </c>
+      <c r="W13">
+        <v>0</v>
+      </c>
+      <c r="X13">
+        <v>0</v>
+      </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
@@ -1096,8 +1524,38 @@
       <c r="N14">
         <v>286</v>
       </c>
+      <c r="O14">
+        <v>132</v>
+      </c>
+      <c r="P14">
+        <v>59</v>
+      </c>
+      <c r="Q14">
+        <v>26</v>
+      </c>
+      <c r="R14">
+        <v>9</v>
+      </c>
+      <c r="S14">
+        <v>2</v>
+      </c>
+      <c r="T14">
+        <v>0</v>
+      </c>
+      <c r="U14">
+        <v>0</v>
+      </c>
+      <c r="V14">
+        <v>0</v>
+      </c>
+      <c r="W14">
+        <v>0</v>
+      </c>
+      <c r="X14">
+        <v>0</v>
+      </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
@@ -1140,8 +1598,38 @@
       <c r="N15">
         <v>373</v>
       </c>
+      <c r="O15">
+        <v>193</v>
+      </c>
+      <c r="P15">
+        <v>105</v>
+      </c>
+      <c r="Q15">
+        <v>59</v>
+      </c>
+      <c r="R15">
+        <v>23</v>
+      </c>
+      <c r="S15">
+        <v>9</v>
+      </c>
+      <c r="T15">
+        <v>5</v>
+      </c>
+      <c r="U15">
+        <v>0</v>
+      </c>
+      <c r="V15">
+        <v>0</v>
+      </c>
+      <c r="W15">
+        <v>0</v>
+      </c>
+      <c r="X15">
+        <v>0</v>
+      </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>18</v>
       </c>
@@ -1184,8 +1672,38 @@
       <c r="N16">
         <v>448</v>
       </c>
+      <c r="O16">
+        <v>208</v>
+      </c>
+      <c r="P16">
+        <v>98</v>
+      </c>
+      <c r="Q16">
+        <v>38</v>
+      </c>
+      <c r="R16">
+        <v>15</v>
+      </c>
+      <c r="S16">
+        <v>7</v>
+      </c>
+      <c r="T16">
+        <v>4</v>
+      </c>
+      <c r="U16">
+        <v>1</v>
+      </c>
+      <c r="V16">
+        <v>0</v>
+      </c>
+      <c r="W16">
+        <v>0</v>
+      </c>
+      <c r="X16">
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>19</v>
       </c>
@@ -1228,13 +1746,43 @@
       <c r="N17">
         <v>179</v>
       </c>
+      <c r="O17">
+        <v>106</v>
+      </c>
+      <c r="P17">
+        <v>61</v>
+      </c>
+      <c r="Q17">
+        <v>33</v>
+      </c>
+      <c r="R17">
+        <v>11</v>
+      </c>
+      <c r="S17">
+        <v>4</v>
+      </c>
+      <c r="T17">
+        <v>1</v>
+      </c>
+      <c r="U17">
+        <v>0</v>
+      </c>
+      <c r="V17">
+        <v>0</v>
+      </c>
+      <c r="W17">
+        <v>0</v>
+      </c>
+      <c r="X17">
+        <v>0</v>
+      </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>21</v>
       </c>
@@ -1244,7 +1792,7 @@
         <v>242597</v>
       </c>
       <c r="D19" s="1">
-        <f t="shared" ref="D19:N19" si="0">SUM(D2:D18)</f>
+        <f t="shared" ref="D19:X19" si="0">SUM(D2:D18)</f>
         <v>229552</v>
       </c>
       <c r="E19" s="1">
@@ -1287,12 +1835,48 @@
         <f t="shared" si="0"/>
         <v>4117</v>
       </c>
-      <c r="P19">
-        <f>SUM(E19:L19)</f>
-        <v>911052</v>
+      <c r="O19" s="1">
+        <f t="shared" si="0"/>
+        <v>2078</v>
+      </c>
+      <c r="P19" s="1">
+        <f t="shared" si="0"/>
+        <v>1017</v>
+      </c>
+      <c r="Q19" s="1">
+        <f t="shared" si="0"/>
+        <v>528</v>
+      </c>
+      <c r="R19" s="1">
+        <f t="shared" si="0"/>
+        <v>278</v>
+      </c>
+      <c r="S19" s="1">
+        <f t="shared" si="0"/>
+        <v>129</v>
+      </c>
+      <c r="T19" s="1">
+        <f t="shared" si="0"/>
+        <v>61</v>
+      </c>
+      <c r="U19" s="1">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="V19" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="W19" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="X19" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E20">
         <f>E19/$D$19</f>
         <v>1</v>
@@ -1330,8 +1914,48 @@
         <v>3.5011674914616299E-2</v>
       </c>
       <c r="N20">
-        <f t="shared" ref="N20" si="5">N19/$D$19</f>
+        <f t="shared" ref="N20:X20" si="5">N19/$D$19</f>
         <v>1.793493413257127E-2</v>
+      </c>
+      <c r="O20">
+        <f t="shared" si="5"/>
+        <v>9.0524151390534609E-3</v>
+      </c>
+      <c r="P20">
+        <f t="shared" si="5"/>
+        <v>4.4303687181989262E-3</v>
+      </c>
+      <c r="Q20">
+        <f t="shared" si="5"/>
+        <v>2.3001324318672892E-3</v>
+      </c>
+      <c r="R20">
+        <f t="shared" si="5"/>
+        <v>1.2110545758695199E-3</v>
+      </c>
+      <c r="S20">
+        <f t="shared" si="5"/>
+        <v>5.6196417369484906E-4</v>
+      </c>
+      <c r="T20">
+        <f t="shared" si="5"/>
+        <v>2.6573499686345577E-4</v>
+      </c>
+      <c r="U20">
+        <f t="shared" si="5"/>
+        <v>7.4057294207848336E-5</v>
+      </c>
+      <c r="V20">
+        <f t="shared" si="5"/>
+        <v>1.7425245695964313E-5</v>
+      </c>
+      <c r="W20">
+        <f t="shared" si="5"/>
+        <v>4.3563114239910783E-6</v>
+      </c>
+      <c r="X20">
+        <f t="shared" si="5"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>